<commit_message>
module 2 finished, carry on with module 3
</commit_message>
<xml_diff>
--- a/exe/2022_FinancialRecords.xlsx
+++ b/exe/2022_FinancialRecords.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\9_Vinager\exe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F7E17F5-446D-4ADE-A58E-FE060F350897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Balance Sheet" sheetId="2" r:id="rId1"/>
@@ -19,25 +18,12 @@
     <sheet name="Records" sheetId="5" r:id="rId4"/>
     <sheet name="Accounts &amp; Wealth" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="191029" concurrentCalc="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="46">
   <si>
     <t>Category</t>
   </si>
@@ -123,6 +109,12 @@
     <t>OPEN</t>
   </si>
   <si>
+    <t>Total Gross Income</t>
+  </si>
+  <si>
+    <t>Cost &amp; Expenses</t>
+  </si>
+  <si>
     <t>Bank Name</t>
   </si>
   <si>
@@ -144,25 +136,28 @@
     <t>Asset Total</t>
   </si>
   <si>
-    <t>Bank Test 1</t>
+    <t>L1</t>
   </si>
   <si>
     <t>Liquid</t>
   </si>
   <si>
-    <t>Bank test 2</t>
-  </si>
-  <si>
-    <t>Fixed 1</t>
+    <t>F1</t>
   </si>
   <si>
     <t>Fixed</t>
   </si>
   <si>
-    <t>Liq1</t>
-  </si>
-  <si>
-    <t>Liq2</t>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>Class 1</t>
+  </si>
+  <si>
+    <t>Class 2</t>
   </si>
   <si>
     <t>Fixed Asset</t>
@@ -171,9 +166,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;€&quot;;\-#,##0.00\ &quot;€&quot;"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
@@ -313,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -331,6 +325,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -340,6 +335,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="5" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -349,9 +345,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -619,42 +612,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.79688" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.19921875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.59765625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.09765625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="18"/>
       <c r="P1" s="2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -701,7 +694,7 @@
         <v>13</v>
       </c>
       <c r="P2" s="4">
-        <f>N7</f>
+        <f>N3</f>
         <v>0</v>
       </c>
       <c r="Q2" s="11"/>
@@ -730,7 +723,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -748,7 +741,9 @@
         <f>SUM(B4:M4)</f>
         <v>0</v>
       </c>
-      <c r="P4" s="6"/>
+      <c r="P4" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
@@ -768,28 +763,31 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
-      <c r="P5" s="12"/>
+      <c r="P5" s="4">
+        <f>N4</f>
+        <v>0</v>
+      </c>
       <c r="Q5" s="12"/>
       <c r="R5" s="12"/>
       <c r="S5" s="12"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="18"/>
       <c r="P6" s="13"/>
       <c r="Q6" s="13"/>
       <c r="R6" s="14"/>
@@ -815,7 +813,9 @@
         <f>SUM(B7:M7)</f>
         <v>0</v>
       </c>
-      <c r="P7" s="13"/>
+      <c r="P7" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="Q7" s="13"/>
       <c r="R7" s="14"/>
       <c r="S7" s="14"/>
@@ -835,7 +835,10 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
-      <c r="P8" s="13"/>
+      <c r="P8" s="4">
+        <f>N7</f>
+        <v>0</v>
+      </c>
       <c r="Q8" s="13"/>
       <c r="R8" s="14"/>
       <c r="S8" s="14"/>
@@ -929,22 +932,22 @@
       <c r="S11" s="14"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="18"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
       <c r="R12" s="14"/>
@@ -999,7 +1002,9 @@
       <c r="S13" s="14"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
+      <c r="A14" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -1019,7 +1024,9 @@
       <c r="S14" s="13"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
+      <c r="A15" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -1039,7 +1046,9 @@
       <c r="S15" s="5"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
+      <c r="A16" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1139,29 +1148,31 @@
       <c r="S20" s="14"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="18"/>
       <c r="P21" s="13"/>
       <c r="Q21" s="13"/>
       <c r="R21" s="14"/>
       <c r="S21" s="14"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
+      <c r="A22" s="8">
+        <f>A14</f>
+      </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -1181,7 +1192,9 @@
       <c r="S22" s="14"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
+      <c r="A23" s="1">
+        <f>A15</f>
+      </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1201,7 +1214,9 @@
       <c r="S23" s="14"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
+      <c r="A24" s="1">
+        <f>A16</f>
+      </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -1221,7 +1236,7 @@
       <c r="S24" s="14"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
+      <c r="A25" s="1"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -1241,7 +1256,7 @@
       <c r="S25" s="14"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
+      <c r="A26" s="1"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -1261,7 +1276,7 @@
       <c r="S26" s="14"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
+      <c r="A27" s="1"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -1665,16 +1680,16 @@
     <mergeCell ref="A21:N21"/>
     <mergeCell ref="A6:N6"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740200000000005" bottom="0.78740200000000005" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.787402" bottom="0.787402" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2130,12 +2145,12 @@
       <c r="N26" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740200000000005" bottom="0.78740200000000005" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.787402" bottom="0.787402" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2592,13 +2607,13 @@
       <c r="N26" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740200000000005" bottom="0.78740200000000005" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.787402" bottom="0.787402" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -2606,7 +2621,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2625,139 +2640,177 @@
       <c r="F1" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="G1" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740200000000005" bottom="0.78740200000000005" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.787402" bottom="0.787402" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:O4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" t="s">
-        <v>29</v>
-      </c>
       <c r="O1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C2">
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="D2">
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I2">
-        <v>400</v>
+        <v>2500</v>
       </c>
       <c r="J2">
-        <v>400</v>
+        <v>2500</v>
       </c>
       <c r="N2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="O2">
-        <v>750</v>
+        <v>3133</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C3">
-        <v>250</v>
+        <v>450</v>
       </c>
       <c r="D3">
-        <v>250</v>
+        <v>450</v>
       </c>
       <c r="H3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="I3">
-        <v>350</v>
+        <v>633</v>
       </c>
       <c r="J3">
-        <v>350</v>
+        <v>633</v>
       </c>
       <c r="N3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O3">
-        <v>2000</v>
+        <v>461</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
         <v>38</v>
       </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
       <c r="C4">
-        <v>2000</v>
+        <v>633</v>
       </c>
       <c r="D4">
-        <v>2000</v>
+        <v>633</v>
       </c>
       <c r="H4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4">
+        <v>461</v>
+      </c>
+      <c r="J4">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>42</v>
       </c>
-      <c r="I4">
-        <v>2000</v>
-      </c>
-      <c r="J4">
-        <v>2000</v>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740200000000005" bottom="0.78740200000000005" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.787402" bottom="0.787402" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Better algorithm when rebordering and clearing needed
</commit_message>
<xml_diff>
--- a/exe/2022_FinancialRecords.xlsx
+++ b/exe/2022_FinancialRecords.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="45">
   <si>
     <t>Income &amp; Expenses</t>
   </si>
@@ -124,22 +124,40 @@
     <t>Account for Transaction</t>
   </si>
   <si>
-    <t>TRK</t>
+    <t>TT1</t>
   </si>
   <si>
     <t>Liquid</t>
   </si>
   <si>
-    <t>PLQ</t>
+    <t>MMR</t>
+  </si>
+  <si>
+    <t>LAP</t>
   </si>
   <si>
     <t>Fixed</t>
   </si>
   <si>
-    <t>VWN</t>
-  </si>
-  <si>
-    <t>PRT</t>
+    <t>TER</t>
+  </si>
+  <si>
+    <t>NAHE</t>
+  </si>
+  <si>
+    <t>MUL</t>
+  </si>
+  <si>
+    <t>Fixed Asset</t>
+  </si>
+  <si>
+    <t>MMA</t>
+  </si>
+  <si>
+    <t>BVE</t>
+  </si>
+  <si>
+    <t>VAGE</t>
   </si>
 </sst>
 </file>
@@ -163,7 +181,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -230,19 +248,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -309,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -317,7 +322,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -327,15 +331,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="6" xfId="0" applyBorder="1"/>
-    <xf borderId="6" xfId="0" applyBorder="1"/>
-    <xf borderId="6" applyBorder="1"/>
+    <xf borderId="5" xfId="0" applyBorder="1"/>
+    <xf borderId="5" xfId="0" applyBorder="1"/>
+    <xf borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -613,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="A15" sqref="A15:N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -625,22 +629,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="10"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="9"/>
     </row>
     <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
@@ -731,43 +735,43 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <f>SUM(Expenses!B:B)</f>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <f>SUM(Expenses!C:C)</f>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <f>SUM(Expenses!D:D)</f>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <f>SUM(Expenses!E:E)</f>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <f>SUM(Expenses!F:F)</f>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <f>SUM(Expenses!G:G)</f>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <f>SUM(Expenses!H:H)</f>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <f>SUM(Expenses!I:I)</f>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="4">
         <f>SUM(Expenses!J:J)</f>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="4">
         <f>SUM(Expenses!K:K)</f>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="4">
         <f>SUM(Expenses!L:L)</f>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="4">
         <f>SUM(Expenses!M:M)</f>
       </c>
       <c r="N4" s="4">
@@ -775,77 +779,77 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.4">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
     </row>
     <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.4">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="10"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="9"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <f>B3+B4</f>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <f>C3+C4</f>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <f>D3+D4</f>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <f>E3+E4</f>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <f>F3+F4</f>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <f>G3+G4</f>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <f>H3+H4</f>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <f>I3+I4</f>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="6">
         <f>J3+J4</f>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="6">
         <f>K3+K4</f>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="6">
         <f>L3+L4</f>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="6">
         <f>M3+M4</f>
       </c>
       <c r="N7" s="4">
@@ -853,39 +857,39 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
     </row>
     <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.4"/>
     <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.4">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="10"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="9"/>
     </row>
     <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
@@ -932,7 +936,9 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="4"/>
+      <c r="A12" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -948,7 +954,9 @@
       <c r="N12" s="4"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
+      <c r="A13" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -963,94 +971,170 @@
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
     </row>
-    <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.4">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-    </row>
-    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.4">
-      <c r="A15" s="8" t="s">
+    <row r="14" spans="1:14">
+      <c r="A14" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+    </row>
+    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.4">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+    </row>
+    <row r="17" spans="1:14" ht="15" x14ac:dyDescent="0.4">
+      <c r="A17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="10"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="9"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="5"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
+      <c r="A18" s="6">
+        <f>A12</f>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" s="4">
+        <f>A13</f>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" s="4">
+        <f>A14</f>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="14">
+        <f>A15</f>
+      </c>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A6:N6"/>
     <mergeCell ref="A10:N10"/>
-    <mergeCell ref="A15:N15"/>
+    <mergeCell ref="A17:N17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.787402" bottom="0.787402" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1058,7 +1142,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
@@ -1071,25 +1155,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="10"/>
-      <c r="G1" s="11" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
+      <c r="G1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="10"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="9"/>
       <c r="L1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1098,8 +1182,8 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.4">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
       <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
@@ -1109,7 +1193,7 @@
       <c r="E2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="12"/>
+      <c r="G2" s="11"/>
       <c r="H2" s="1" t="s">
         <v>25</v>
       </c>
@@ -1119,8 +1203,12 @@
       <c r="J2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
+      <c r="L2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="4">
+        <v>1010</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -1129,83 +1217,110 @@
       <c r="B3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="5">
-        <v>225</v>
-      </c>
-      <c r="D3" s="5">
-        <v>225</v>
+      <c r="C3" s="4">
+        <v>450</v>
+      </c>
+      <c r="D3" s="4">
+        <v>450</v>
       </c>
       <c r="E3" s="4">
         <f>D3-C3</f>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="4"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
+      <c r="G3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="4">
+        <v>235</v>
+      </c>
+      <c r="I3" s="4">
+        <v>235</v>
+      </c>
+      <c r="J3" s="4">
+        <f>I3-H3</f>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="4">
+        <v>245</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="4">
+        <v>560</v>
+      </c>
+      <c r="D4" s="4">
+        <v>560</v>
+      </c>
+      <c r="E4" s="4">
+        <f>D4-C4</f>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="4">
+        <v>235</v>
+      </c>
+      <c r="I4" s="4">
+        <v>235</v>
+      </c>
+      <c r="J4" s="4">
+        <f>I4-H4</f>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="5">
-        <v>250</v>
-      </c>
-      <c r="D4" s="5">
-        <v>250</v>
-      </c>
-      <c r="E4" s="5">
-        <f>D4-C4</f>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="13">
+      <c r="C5" s="12">
         <v>245</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>245</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <f>D5-C5</f>
       </c>
+      <c r="G5" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="14">
+        <v>540</v>
+      </c>
+      <c r="I5" s="14">
+        <v>540</v>
+      </c>
+      <c r="J5" s="14">
+        <f>I5-H5</f>
+      </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="14">
-        <v>456</v>
-      </c>
-      <c r="D6" s="14">
-        <v>456</v>
-      </c>
-      <c r="E6" s="14">
-        <f>D6-C6</f>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="G6" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="14">
+        <v>245</v>
+      </c>
+      <c r="I6" s="14">
+        <v>245</v>
+      </c>
+      <c r="J6" s="14">
+        <f>I6-H6</f>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1290,36 +1405,36 @@
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.787402" bottom="0.787402" header="0.3" footer="0.3"/>
@@ -1397,36 +1512,36 @@
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.787402" bottom="0.787402" header="0.3" footer="0.3"/>
@@ -1475,12 +1590,12 @@
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.787402" bottom="0.787402" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add function to get Accounts and Wealth in utils.cpp
-implemented on wealth allocation
-start implementing update sheet
</commit_message>
<xml_diff>
--- a/exe/2022_FinancialRecords.xlsx
+++ b/exe/2022_FinancialRecords.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="49">
   <si>
     <t>Income &amp; Expenses</t>
   </si>
@@ -124,55 +124,52 @@
     <t>Account for Transaction</t>
   </si>
   <si>
-    <t>A</t>
+    <t>AMAR</t>
   </si>
   <si>
     <t>Liquid</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>MER</t>
+    <t>MEGA</t>
   </si>
   <si>
     <t>Fixed</t>
   </si>
   <si>
-    <t>LAP</t>
-  </si>
-  <si>
-    <t>MEN</t>
-  </si>
-  <si>
-    <t>PAL</t>
-  </si>
-  <si>
-    <t>GERO</t>
+    <t>LERO</t>
+  </si>
+  <si>
+    <t>PLAO</t>
+  </si>
+  <si>
+    <t>LLA</t>
+  </si>
+  <si>
+    <t>MNE</t>
   </si>
   <si>
     <t>Fixed Asset</t>
   </si>
   <si>
-    <t>AA</t>
-  </si>
-  <si>
-    <t>PLL</t>
-  </si>
-  <si>
-    <t>MMEN</t>
-  </si>
-  <si>
-    <t>MMAL</t>
-  </si>
-  <si>
-    <t>PEO</t>
-  </si>
-  <si>
-    <t>GHA</t>
+    <t>HAMA</t>
+  </si>
+  <si>
+    <t>MERO</t>
+  </si>
+  <si>
+    <t>TORI</t>
+  </si>
+  <si>
+    <t>LAH</t>
+  </si>
+  <si>
+    <t>MARC</t>
+  </si>
+  <si>
+    <t>HATO</t>
+  </si>
+  <si>
+    <t>NHA</t>
   </si>
 </sst>
 </file>
@@ -348,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -374,6 +371,7 @@
     </xf>
     <xf borderId="6" xfId="0" applyBorder="1"/>
     <xf borderId="6" xfId="0" applyBorder="1"/>
+    <xf borderId="11" xfId="0" applyBorder="1"/>
     <xf borderId="11" xfId="0" applyBorder="1"/>
     <xf borderId="11" applyBorder="1"/>
   </cellXfs>
@@ -1163,7 +1161,7 @@
         <v>34</v>
       </c>
       <c r="M2" s="4">
-        <v>815</v>
+        <v>800</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -1174,10 +1172,10 @@
         <v>34</v>
       </c>
       <c r="C3" s="5">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="D3" s="5">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="E3" s="4">
         <f>D3-C3</f>
@@ -1186,19 +1184,19 @@
         <v>46</v>
       </c>
       <c r="H3" s="5">
-        <v>225</v>
+        <v>300</v>
       </c>
       <c r="I3" s="5">
-        <v>225</v>
+        <v>300</v>
       </c>
       <c r="J3" s="4">
         <f>I3-H3</f>
       </c>
       <c r="L3" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M3" s="5">
-        <v>234</v>
+        <v>475</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
@@ -1206,102 +1204,89 @@
         <v>35</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C4" s="5">
-        <v>125</v>
+        <v>250</v>
       </c>
       <c r="D4" s="5">
-        <v>125</v>
+        <v>250</v>
       </c>
       <c r="E4" s="5">
         <f>D4-C4</f>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="5">
-        <v>125</v>
-      </c>
-      <c r="I4" s="5">
-        <v>125</v>
-      </c>
-      <c r="J4" s="5">
+      <c r="H4" s="17">
+        <v>350</v>
+      </c>
+      <c r="I4" s="17">
+        <v>350</v>
+      </c>
+      <c r="J4" s="17">
         <f>I4-H4</f>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>34</v>
-      </c>
       <c r="C5" s="13">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="D5" s="13">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="E5" s="13">
         <f>D5-C5</f>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="15">
-        <v>250</v>
-      </c>
-      <c r="I5" s="15">
-        <v>250</v>
-      </c>
-      <c r="J5" s="15">
+      <c r="H5" s="17">
+        <v>150</v>
+      </c>
+      <c r="I5" s="17">
+        <v>150</v>
+      </c>
+      <c r="J5" s="17">
         <f>I5-H5</f>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C6" s="14">
-        <v>234</v>
+        <v>350</v>
       </c>
       <c r="D6" s="14">
-        <v>234</v>
+        <v>350</v>
       </c>
       <c r="E6" s="14">
         <f>D6-C6</f>
       </c>
-      <c r="G6" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="16">
-        <v>215</v>
-      </c>
-      <c r="I6" s="16">
-        <v>215</v>
-      </c>
-      <c r="J6" s="16">
+      <c r="G6" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="17">
+        <v>475</v>
+      </c>
+      <c r="I6" s="17">
+        <v>475</v>
+      </c>
+      <c r="J6" s="17">
         <f>I6-H6</f>
       </c>
     </row>
-    <row r="7" spans="1:13">
-      <c r="G7" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="16">
-        <v>234</v>
-      </c>
-      <c r="I7" s="16">
-        <v>234</v>
-      </c>
-      <c r="J7" s="16">
-        <f>I7-H7</f>
-      </c>
-    </row>
+    <row r="7" spans="1:13"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:A2"/>

</xml_diff>

<commit_message>
implement adding accounts code in Records sheet
-Next: implement automatic adjustment in Financial Statement sheet for the wealth class
</commit_message>
<xml_diff>
--- a/exe/2022_FinancialRecords.xlsx
+++ b/exe/2022_FinancialRecords.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="53">
   <si>
     <t>Income &amp; Expenses</t>
   </si>
@@ -124,52 +124,64 @@
     <t>Account for Transaction</t>
   </si>
   <si>
-    <t>AMAR</t>
+    <t>A</t>
   </si>
   <si>
     <t>Liquid</t>
   </si>
   <si>
-    <t>MEGA</t>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>MER</t>
   </si>
   <si>
     <t>Fixed</t>
   </si>
   <si>
-    <t>LERO</t>
-  </si>
-  <si>
-    <t>PLAO</t>
-  </si>
-  <si>
-    <t>LLA</t>
-  </si>
-  <si>
-    <t>MNE</t>
+    <t>LAP</t>
+  </si>
+  <si>
+    <t>MEN</t>
+  </si>
+  <si>
+    <t>PAL</t>
+  </si>
+  <si>
+    <t>GERO</t>
   </si>
   <si>
     <t>Fixed Asset</t>
   </si>
   <si>
-    <t>HAMA</t>
-  </si>
-  <si>
-    <t>MERO</t>
-  </si>
-  <si>
-    <t>TORI</t>
-  </si>
-  <si>
-    <t>LAH</t>
-  </si>
-  <si>
-    <t>MARC</t>
-  </si>
-  <si>
-    <t>HATO</t>
-  </si>
-  <si>
-    <t>NHA</t>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>PLL</t>
+  </si>
+  <si>
+    <t>MMEN</t>
+  </si>
+  <si>
+    <t>MMAL</t>
+  </si>
+  <si>
+    <t>PEO</t>
+  </si>
+  <si>
+    <t>GHA</t>
+  </si>
+  <si>
+    <t>MMN</t>
+  </si>
+  <si>
+    <t>LAE</t>
+  </si>
+  <si>
+    <t>PPAL</t>
   </si>
 </sst>
 </file>
@@ -345,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -373,7 +385,9 @@
     <xf borderId="6" xfId="0" applyBorder="1"/>
     <xf borderId="11" xfId="0" applyBorder="1"/>
     <xf borderId="11" xfId="0" applyBorder="1"/>
-    <xf borderId="11" applyBorder="1"/>
+    <xf borderId="11" xfId="0" applyBorder="1"/>
+    <xf borderId="4" applyBorder="1"/>
+    <xf borderId="5" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1161,7 +1175,7 @@
         <v>34</v>
       </c>
       <c r="M2" s="4">
-        <v>800</v>
+        <v>815</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -1172,31 +1186,31 @@
         <v>34</v>
       </c>
       <c r="C3" s="5">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="D3" s="5">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="E3" s="4">
         <f>D3-C3</f>
       </c>
       <c r="G3" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H3" s="5">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="I3" s="5">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="J3" s="4">
         <f>I3-H3</f>
       </c>
       <c r="L3" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="M3" s="5">
-        <v>475</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
@@ -1204,25 +1218,25 @@
         <v>35</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" s="5">
-        <v>250</v>
+        <v>125</v>
       </c>
       <c r="D4" s="5">
-        <v>250</v>
+        <v>125</v>
       </c>
       <c r="E4" s="5">
         <f>D4-C4</f>
       </c>
       <c r="G4" s="17" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H4" s="17">
-        <v>350</v>
+        <v>250</v>
       </c>
       <c r="I4" s="17">
-        <v>350</v>
+        <v>250</v>
       </c>
       <c r="J4" s="17">
         <f>I4-H4</f>
@@ -1230,28 +1244,28 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C5" s="13">
-        <v>225</v>
+        <v>245</v>
       </c>
       <c r="D5" s="13">
-        <v>225</v>
+        <v>245</v>
       </c>
       <c r="E5" s="13">
         <f>D5-C5</f>
       </c>
       <c r="G5" s="17" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H5" s="17">
-        <v>150</v>
+        <v>315</v>
       </c>
       <c r="I5" s="17">
-        <v>150</v>
+        <v>315</v>
       </c>
       <c r="J5" s="17">
         <f>I5-H5</f>
@@ -1259,28 +1273,28 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>34</v>
-      </c>
       <c r="C6" s="14">
-        <v>350</v>
+        <v>234</v>
       </c>
       <c r="D6" s="14">
-        <v>350</v>
+        <v>234</v>
       </c>
       <c r="E6" s="14">
         <f>D6-C6</f>
       </c>
       <c r="G6" s="17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H6" s="17">
-        <v>475</v>
+        <v>234</v>
       </c>
       <c r="I6" s="17">
-        <v>475</v>
+        <v>234</v>
       </c>
       <c r="J6" s="17">
         <f>I6-H6</f>
@@ -1515,7 +1529,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
@@ -1526,7 +1540,7 @@
     <col min="6" max="6" width="20.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -1545,16 +1559,32 @@
       <c r="F1" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>

</xml_diff>

<commit_message>
implemented automatic addition of wealth class in FIinancial Statement
-next: code for case missing_rows < 1: wealth class reduced
-test the code in case wealth class added from 4 to 5
</commit_message>
<xml_diff>
--- a/exe/2022_FinancialRecords.xlsx
+++ b/exe/2022_FinancialRecords.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="53">
   <si>
     <t>Income &amp; Expenses</t>
   </si>
@@ -357,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -388,6 +388,7 @@
     <xf borderId="11" xfId="0" applyBorder="1"/>
     <xf borderId="4" applyBorder="1"/>
     <xf borderId="5" applyBorder="1"/>
+    <xf borderId="11" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -665,7 +666,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A15" sqref="A15:N15"/>
@@ -984,7 +985,9 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="4"/>
+      <c r="A12" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -999,110 +1002,172 @@
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-    </row>
-    <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.4">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-    </row>
-    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.4">
-      <c r="A15" s="8" t="s">
+    <row r="13" spans="1:14">
+      <c r="A13" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+    </row>
+    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.4">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+    </row>
+    <row r="17" spans="1:14" ht="15" x14ac:dyDescent="0.4">
+      <c r="A17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="10"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="10"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="5"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
+      <c r="A18" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A6:N6"/>
     <mergeCell ref="A10:N10"/>
-    <mergeCell ref="A15:N15"/>
+    <mergeCell ref="A17:N17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.787402" bottom="0.787402" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Bug for addition wealth class fixed
-test for reduction of wealth class
</commit_message>
<xml_diff>
--- a/exe/2022_FinancialRecords.xlsx
+++ b/exe/2022_FinancialRecords.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="56">
   <si>
     <t>Income &amp; Expenses</t>
   </si>
@@ -182,6 +182,15 @@
   </si>
   <si>
     <t>PPAL</t>
+  </si>
+  <si>
+    <t>LLA</t>
+  </si>
+  <si>
+    <t>HH</t>
+  </si>
+  <si>
+    <t>ZUT</t>
   </si>
 </sst>
 </file>
@@ -357,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -386,8 +395,10 @@
     <xf borderId="11" xfId="0" applyBorder="1"/>
     <xf borderId="11" xfId="0" applyBorder="1"/>
     <xf borderId="11" xfId="0" applyBorder="1"/>
-    <xf borderId="4" applyBorder="1"/>
-    <xf borderId="5" applyBorder="1"/>
+    <xf borderId="4" xfId="0" applyBorder="1"/>
+    <xf borderId="5" xfId="0" applyBorder="1"/>
+    <xf borderId="11" xfId="0" applyBorder="1"/>
+    <xf borderId="11" xfId="0" applyBorder="1"/>
     <xf borderId="11" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -666,7 +677,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A15" sqref="A15:N15"/>
@@ -986,7 +997,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1004,7 +1015,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="20" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B13" s="20"/>
       <c r="C13" s="20"/>
@@ -1022,7 +1033,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B14" s="20"/>
       <c r="C14" s="20"/>
@@ -1040,7 +1051,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1056,118 +1067,190 @@
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
     </row>
-    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.4">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-    </row>
-    <row r="17" spans="1:14" ht="15" x14ac:dyDescent="0.4">
-      <c r="A17" s="8" t="s">
+    <row r="16" spans="1:14">
+      <c r="A16" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+    </row>
+    <row r="18" spans="1:14" ht="15" x14ac:dyDescent="0.4">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+    </row>
+    <row r="19" spans="1:14" ht="15" x14ac:dyDescent="0.4">
+      <c r="A19" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="10"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="10"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="20" t="s">
+      <c r="A20" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="20"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A6:N6"/>
     <mergeCell ref="A10:N10"/>
-    <mergeCell ref="A17:N17"/>
+    <mergeCell ref="A19:N19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.787402" bottom="0.787402" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1175,7 +1258,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
@@ -1260,13 +1343,13 @@
         <f>D3-C3</f>
       </c>
       <c r="G3" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H3" s="5">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="I3" s="5">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="J3" s="4">
         <f>I3-H3</f>
@@ -1294,16 +1377,16 @@
       <c r="E4" s="5">
         <f>D4-C4</f>
       </c>
-      <c r="G4" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="H4" s="17">
-        <v>250</v>
-      </c>
-      <c r="I4" s="17">
-        <v>250</v>
-      </c>
-      <c r="J4" s="17">
+      <c r="G4" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="21">
+        <v>350</v>
+      </c>
+      <c r="I4" s="21">
+        <v>350</v>
+      </c>
+      <c r="J4" s="21">
         <f>I4-H4</f>
       </c>
     </row>
@@ -1323,16 +1406,16 @@
       <c r="E5" s="13">
         <f>D5-C5</f>
       </c>
-      <c r="G5" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="H5" s="17">
-        <v>315</v>
-      </c>
-      <c r="I5" s="17">
-        <v>315</v>
-      </c>
-      <c r="J5" s="17">
+      <c r="G5" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="21">
+        <v>120</v>
+      </c>
+      <c r="I5" s="21">
+        <v>120</v>
+      </c>
+      <c r="J5" s="21">
         <f>I5-H5</f>
       </c>
     </row>
@@ -1352,20 +1435,47 @@
       <c r="E6" s="14">
         <f>D6-C6</f>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="21">
+        <v>40</v>
+      </c>
+      <c r="I6" s="21">
+        <v>40</v>
+      </c>
+      <c r="J6" s="21">
+        <f>I6-H6</f>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="G7" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="21">
+        <v>85</v>
+      </c>
+      <c r="I7" s="21">
+        <v>85</v>
+      </c>
+      <c r="J7" s="21">
+        <f>I7-H7</f>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="G8" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H8" s="21">
         <v>234</v>
       </c>
-      <c r="I6" s="17">
+      <c r="I8" s="21">
         <v>234</v>
       </c>
-      <c r="J6" s="17">
-        <f>I6-H6</f>
-      </c>
-    </row>
-    <row r="7" spans="1:13"/>
+      <c r="J8" s="21">
+        <f>I8-H8</f>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:A2"/>

</xml_diff>

<commit_message>
Module 2.3 bug free
-next: start the transaction calculator
</commit_message>
<xml_diff>
--- a/exe/2022_FinancialRecords.xlsx
+++ b/exe/2022_FinancialRecords.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="58">
   <si>
     <t>Income &amp; Expenses</t>
   </si>
@@ -191,6 +191,12 @@
   </si>
   <si>
     <t>ZUT</t>
+  </si>
+  <si>
+    <t>APER</t>
+  </si>
+  <si>
+    <t>MENDA</t>
   </si>
 </sst>
 </file>
@@ -366,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -399,7 +405,8 @@
     <xf borderId="5" xfId="0" applyBorder="1"/>
     <xf borderId="11" xfId="0" applyBorder="1"/>
     <xf borderId="11" xfId="0" applyBorder="1"/>
-    <xf borderId="11" applyBorder="1"/>
+    <xf borderId="11" xfId="0" applyBorder="1"/>
+    <xf borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -677,7 +684,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A15" sqref="A15:N15"/>
@@ -997,7 +1004,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1015,7 +1022,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="20" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B13" s="20"/>
       <c r="C13" s="20"/>
@@ -1032,225 +1039,117 @@
       <c r="N13" s="20"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22"/>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="A17" s="22" t="s">
+      <c r="A14" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-    </row>
-    <row r="18" spans="1:14" ht="15" x14ac:dyDescent="0.4">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-    </row>
-    <row r="19" spans="1:14" ht="15" x14ac:dyDescent="0.4">
-      <c r="A19" s="8" t="s">
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+    </row>
+    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.4">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+    </row>
+    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.4">
+      <c r="A16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="10"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="20"/>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
-    </row>
-    <row r="25" spans="1:14">
-      <c r="A25" s="22" t="s">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="10"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A6:N6"/>
     <mergeCell ref="A10:N10"/>
-    <mergeCell ref="A19:N19"/>
+    <mergeCell ref="A16:N16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.787402" bottom="0.787402" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1343,13 +1242,13 @@
         <f>D3-C3</f>
       </c>
       <c r="G3" s="4" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="H3" s="5">
-        <v>220</v>
+        <v>550</v>
       </c>
       <c r="I3" s="5">
-        <v>220</v>
+        <v>550</v>
       </c>
       <c r="J3" s="4">
         <f>I3-H3</f>
@@ -1377,16 +1276,16 @@
       <c r="E4" s="5">
         <f>D4-C4</f>
       </c>
-      <c r="G4" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="21">
-        <v>350</v>
-      </c>
-      <c r="I4" s="21">
-        <v>350</v>
-      </c>
-      <c r="J4" s="21">
+      <c r="G4" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="23">
+        <v>265</v>
+      </c>
+      <c r="I4" s="23">
+        <v>265</v>
+      </c>
+      <c r="J4" s="23">
         <f>I4-H4</f>
       </c>
     </row>
@@ -1406,16 +1305,16 @@
       <c r="E5" s="13">
         <f>D5-C5</f>
       </c>
-      <c r="G5" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="21">
-        <v>120</v>
-      </c>
-      <c r="I5" s="21">
-        <v>120</v>
-      </c>
-      <c r="J5" s="21">
+      <c r="G5" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="23">
+        <v>234</v>
+      </c>
+      <c r="I5" s="23">
+        <v>234</v>
+      </c>
+      <c r="J5" s="23">
         <f>I5-H5</f>
       </c>
     </row>
@@ -1435,47 +1334,9 @@
       <c r="E6" s="14">
         <f>D6-C6</f>
       </c>
-      <c r="G6" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="H6" s="21">
-        <v>40</v>
-      </c>
-      <c r="I6" s="21">
-        <v>40</v>
-      </c>
-      <c r="J6" s="21">
-        <f>I6-H6</f>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="G7" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="H7" s="21">
-        <v>85</v>
-      </c>
-      <c r="I7" s="21">
-        <v>85</v>
-      </c>
-      <c r="J7" s="21">
-        <f>I7-H7</f>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="G8" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="21">
-        <v>234</v>
-      </c>
-      <c r="I8" s="21">
-        <v>234</v>
-      </c>
-      <c r="J8" s="21">
-        <f>I8-H8</f>
-      </c>
-    </row>
+    </row>
+    <row r="7" spans="1:13"/>
+    <row r="8" spans="1:13"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:A2"/>

</xml_diff>

<commit_message>
Cleaner input validity checks
-continue transaction processing
</commit_message>
<xml_diff>
--- a/exe/2022_FinancialRecords.xlsx
+++ b/exe/2022_FinancialRecords.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="58">
   <si>
     <t>Income &amp; Expenses</t>
   </si>
@@ -406,7 +406,7 @@
     <xf borderId="11" xfId="0" applyBorder="1"/>
     <xf borderId="11" xfId="0" applyBorder="1"/>
     <xf borderId="11" xfId="0" applyBorder="1"/>
-    <xf borderId="11" xfId="0" applyBorder="1"/>
+    <xf borderId="11" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -684,7 +684,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A15" sqref="A15:N15"/>
@@ -1004,7 +1004,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1022,7 +1022,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="20" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B13" s="20"/>
       <c r="C13" s="20"/>
@@ -1039,117 +1039,225 @@
       <c r="N13" s="20"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
-    </row>
-    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.4">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-    </row>
-    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.4">
-      <c r="A16" s="8" t="s">
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+    </row>
+    <row r="18" spans="1:14" ht="15" x14ac:dyDescent="0.4">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+    </row>
+    <row r="19" spans="1:14" ht="15" x14ac:dyDescent="0.4">
+      <c r="A19" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="10"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="10"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="20"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A6:N6"/>
     <mergeCell ref="A10:N10"/>
-    <mergeCell ref="A16:N16"/>
+    <mergeCell ref="A19:N19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.787402" bottom="0.787402" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Interaccount Transaction On The Way
-input successful, but destroy borders on some sheets
</commit_message>
<xml_diff>
--- a/exe/2022_FinancialRecords.xlsx
+++ b/exe/2022_FinancialRecords.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>Category</t>
   </si>
@@ -177,12 +177,36 @@
   </si>
   <si>
     <t>Nakata</t>
+  </si>
+  <si>
+    <t>Nagatomo</t>
+  </si>
+  <si>
+    <t>Ventradate</t>
+  </si>
+  <si>
+    <t>Geverine</t>
+  </si>
+  <si>
+    <t>Starting Point</t>
+  </si>
+  <si>
+    <t>Test 1</t>
+  </si>
+  <si>
+    <t>Begarnade to Cernique</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="167" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="0">
     <font>
       <sz val="11"/>
@@ -363,13 +387,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -394,7 +416,13 @@
     <xf borderId="12" xfId="0" applyBorder="1"/>
     <xf borderId="12" xfId="0" applyBorder="1"/>
     <xf borderId="12" xfId="0" applyBorder="1"/>
-    <xf borderId="12" applyBorder="1"/>
+    <xf borderId="12" xfId="0" applyBorder="1"/>
+    <xf borderId="12" xfId="0" applyBorder="1"/>
+    <xf borderId="4" xfId="0" applyBorder="1"/>
+    <xf borderId="5" xfId="0" applyBorder="1"/>
+    <xf borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -684,22 +712,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="12"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="10"/>
     </row>
     <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -746,418 +774,418 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="12"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="10"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="4">
+      <c r="A4" s="0"/>
+      <c r="B4" s="0"/>
+      <c r="C4" s="0"/>
+      <c r="D4" s="0"/>
+      <c r="E4" s="0"/>
+      <c r="F4" s="0"/>
+      <c r="G4" s="0"/>
+      <c r="H4" s="0"/>
+      <c r="I4" s="0"/>
+      <c r="J4" s="0"/>
+      <c r="K4" s="0"/>
+      <c r="L4" s="0"/>
+      <c r="M4" s="0"/>
+      <c r="N4" s="0">
         <f>SUM(B4:M4)</f>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
+      <c r="A5" s="0"/>
+      <c r="B5" s="0"/>
+      <c r="C5" s="0"/>
+      <c r="D5" s="0"/>
+      <c r="E5" s="0"/>
+      <c r="F5" s="0"/>
+      <c r="G5" s="0"/>
+      <c r="H5" s="0"/>
+      <c r="I5" s="0"/>
+      <c r="J5" s="0"/>
+      <c r="K5" s="0"/>
+      <c r="L5" s="0"/>
+      <c r="M5" s="0"/>
+      <c r="N5" s="0"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
+      <c r="A6" s="0"/>
+      <c r="B6" s="0"/>
+      <c r="C6" s="0"/>
+      <c r="D6" s="0"/>
+      <c r="E6" s="0"/>
+      <c r="F6" s="0"/>
+      <c r="G6" s="0"/>
+      <c r="H6" s="0"/>
+      <c r="I6" s="0"/>
+      <c r="J6" s="0"/>
+      <c r="K6" s="0"/>
+      <c r="L6" s="0"/>
+      <c r="M6" s="0"/>
+      <c r="N6" s="0"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
+      <c r="A7" s="0"/>
+      <c r="B7" s="0"/>
+      <c r="C7" s="0"/>
+      <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
+      <c r="F7" s="0"/>
+      <c r="G7" s="0"/>
+      <c r="H7" s="0"/>
+      <c r="I7" s="0"/>
+      <c r="J7" s="0"/>
+      <c r="K7" s="0"/>
+      <c r="L7" s="0"/>
+      <c r="M7" s="0"/>
+      <c r="N7" s="0"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
+      <c r="A8" s="0"/>
+      <c r="B8" s="0"/>
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
+      <c r="F8" s="0"/>
+      <c r="G8" s="0"/>
+      <c r="H8" s="0"/>
+      <c r="I8" s="0"/>
+      <c r="J8" s="0"/>
+      <c r="K8" s="0"/>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
+      <c r="N8" s="0"/>
     </row>
     <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
+      <c r="A9" s="0"/>
+      <c r="B9" s="0"/>
+      <c r="C9" s="0"/>
+      <c r="D9" s="0"/>
+      <c r="E9" s="0"/>
+      <c r="F9" s="0"/>
+      <c r="G9" s="0"/>
+      <c r="H9" s="0"/>
+      <c r="I9" s="0"/>
+      <c r="J9" s="0"/>
+      <c r="K9" s="0"/>
+      <c r="L9" s="0"/>
+      <c r="M9" s="0"/>
+      <c r="N9" s="0"/>
     </row>
     <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.35">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="12"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="10"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="4">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="0">
         <f>SUM(B11:M11)</f>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
+      <c r="A12" s="0"/>
+      <c r="B12" s="0"/>
+      <c r="C12" s="0"/>
+      <c r="D12" s="0"/>
+      <c r="E12" s="0"/>
+      <c r="F12" s="0"/>
+      <c r="G12" s="0"/>
+      <c r="H12" s="0"/>
+      <c r="I12" s="0"/>
+      <c r="J12" s="0"/>
+      <c r="K12" s="0"/>
+      <c r="L12" s="0"/>
+      <c r="M12" s="0"/>
+      <c r="N12" s="0"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
+      <c r="A13" s="0"/>
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
+      <c r="D13" s="0"/>
+      <c r="E13" s="0"/>
+      <c r="F13" s="0"/>
+      <c r="G13" s="0"/>
+      <c r="H13" s="0"/>
+      <c r="I13" s="0"/>
+      <c r="J13" s="0"/>
+      <c r="K13" s="0"/>
+      <c r="L13" s="0"/>
+      <c r="M13" s="0"/>
+      <c r="N13" s="0"/>
     </row>
     <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
+      <c r="A14" s="0"/>
+      <c r="B14" s="0"/>
+      <c r="C14" s="0"/>
+      <c r="D14" s="0"/>
+      <c r="E14" s="0"/>
+      <c r="F14" s="0"/>
+      <c r="G14" s="0"/>
+      <c r="H14" s="0"/>
+      <c r="I14" s="0"/>
+      <c r="J14" s="0"/>
+      <c r="K14" s="0"/>
+      <c r="L14" s="0"/>
+      <c r="M14" s="0"/>
+      <c r="N14" s="0"/>
     </row>
     <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.35">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="12"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="10"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="0">
         <f>SUM(B4:B8)</f>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="0">
         <f>SUM(C4:C8)</f>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="0">
         <f>SUM(D4:D8)</f>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="0">
         <f>SUM(E4:E8)</f>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="0">
         <f>SUM(F4:F8)</f>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="0">
         <f>SUM(G4:G8)</f>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="0">
         <f>SUM(H4:H8)</f>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="0">
         <f>SUM(I4:I8)</f>
       </c>
-      <c r="J16" s="4">
+      <c r="J16" s="0">
         <f>SUM(J4:J8)</f>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="0">
         <f>SUM(K4:K8)</f>
       </c>
-      <c r="L16" s="4">
+      <c r="L16" s="0">
         <f>SUM(L4:L8)</f>
       </c>
-      <c r="M16" s="4">
+      <c r="M16" s="0">
         <f>SUM(M4:M8)</f>
       </c>
-      <c r="N16" s="4">
+      <c r="N16" s="0">
         <f>SUM(B16:M16)</f>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="0">
         <f>SUM(B10:B14)</f>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="0">
         <f>SUM(C10:C14)</f>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="0">
         <f>SUM(D10:D14)</f>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="0">
         <f>SUM(E10:E14)</f>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="0">
         <f>SUM(F10:F14)</f>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="0">
         <f>SUM(G10:G14)</f>
       </c>
-      <c r="H17" s="5">
+      <c r="H17" s="0">
         <f>SUM(H10:H14)</f>
       </c>
-      <c r="I17" s="5">
+      <c r="I17" s="0">
         <f>SUM(I10:I14)</f>
       </c>
-      <c r="J17" s="5">
+      <c r="J17" s="0">
         <f>SUM(J10:J14)</f>
       </c>
-      <c r="K17" s="5">
+      <c r="K17" s="0">
         <f>SUM(K10:K14)</f>
       </c>
-      <c r="L17" s="5">
+      <c r="L17" s="0">
         <f>SUM(L10:L14)</f>
       </c>
-      <c r="M17" s="5">
+      <c r="M17" s="0">
         <f>SUM(M10:M14)</f>
       </c>
-      <c r="N17" s="4">
+      <c r="N17" s="0">
         <f>SUM(B17:M17)</f>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="4">
         <f>B16+B17</f>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="4">
         <f>C16+C17</f>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="4">
         <f>D16+D17</f>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="4">
         <f>E16+E17</f>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="4">
         <f>F16+F17</f>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="4">
         <f>G16+G17</f>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="4">
         <f>H16+H17</f>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="4">
         <f>I16+I17</f>
       </c>
-      <c r="J18" s="6">
+      <c r="J18" s="4">
         <f>J16+J17</f>
       </c>
-      <c r="K18" s="6">
+      <c r="K18" s="4">
         <f>K16+K17</f>
       </c>
-      <c r="L18" s="6">
+      <c r="L18" s="4">
         <f>L16+L17</f>
       </c>
-      <c r="M18" s="6">
+      <c r="M18" s="4">
         <f>M16+M17</f>
       </c>
-      <c r="N18" s="9">
+      <c r="N18" s="7">
         <f>SUM(B18:M18)</f>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
+      <c r="A19" s="0"/>
+      <c r="B19" s="0"/>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0"/>
+      <c r="E19" s="0"/>
+      <c r="F19" s="0"/>
+      <c r="G19" s="0"/>
+      <c r="H19" s="0"/>
+      <c r="I19" s="0"/>
+      <c r="J19" s="0"/>
+      <c r="K19" s="0"/>
+      <c r="L19" s="0"/>
+      <c r="M19" s="0"/>
+      <c r="N19" s="0"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1185,28 +1213,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="12"/>
-      <c r="G1" s="13" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="10"/>
+      <c r="G1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="11"/>
-      <c r="K1" s="12"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="10"/>
       <c r="M1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1215,8 +1243,8 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.35">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
       <c r="C2" s="1" t="s">
         <v>22</v>
       </c>
@@ -1226,8 +1254,8 @@
       <c r="E2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
       <c r="I2" s="1" t="s">
         <v>22</v>
       </c>
@@ -1237,116 +1265,133 @@
       <c r="K2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="0">
         <v>1250</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="0">
         <v>500</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="0">
         <v>500</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="0">
         <f>D3-C3</f>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" s="4">
-        <v>57.5</v>
-      </c>
-      <c r="I3" s="5">
-        <v>718.75</v>
-      </c>
-      <c r="J3" s="5">
+      <c r="G3" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="0">
+        <v>35.7</v>
+      </c>
+      <c r="I3" s="0">
+        <v>446.25</v>
+      </c>
+      <c r="J3" s="0">
         <f>H3/100 * N2</f>
-      </c>
-      <c r="K3" s="4">
+        <v>446.25</v>
+      </c>
+      <c r="K3" s="0">
         <f>J3-I3</f>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="0">
         <v>400</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="0">
         <v>750</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="0">
         <v>750</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="0">
         <f>D4-C4</f>
       </c>
-      <c r="G4" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="20">
-        <v>42.5</v>
-      </c>
-      <c r="I4" s="20">
-        <v>531.25</v>
-      </c>
-      <c r="J4" s="20">
-        <f>H4/100 * N2</f>
-      </c>
-      <c r="K4" s="20">
+      <c r="G4" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="19">
+        <v>25.3</v>
+      </c>
+      <c r="I4" s="19">
+        <v>316.25</v>
+      </c>
+      <c r="J4" s="19">
+        <v>316.25</v>
+      </c>
+      <c r="K4" s="19">
         <f>J4-I4</f>
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="13">
         <v>400</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="13">
         <v>400</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="13">
         <f>D5-C5</f>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="19">
+        <v>39</v>
+      </c>
+      <c r="I5" s="19">
+        <v>487.5</v>
+      </c>
+      <c r="J5" s="19">
+        <v>487.5</v>
+      </c>
+      <c r="K5" s="19">
+        <f>J5-I5</f>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="G6" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H6" s="19">
         <v>100</v>
       </c>
-      <c r="I5" s="20">
+      <c r="I6" s="19">
         <v>400</v>
       </c>
-      <c r="J5" s="20">
-        <f>N3</f>
-      </c>
-      <c r="K5" s="20">
-        <f>J5-I5</f>
-      </c>
-    </row>
-    <row r="6" spans="1:14"/>
+      <c r="J6" s="19">
+        <v>400</v>
+      </c>
+      <c r="K6" s="19">
+        <f>J6-I6</f>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A1:A2"/>
@@ -1362,7 +1407,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
@@ -1373,7 +1418,7 @@
     <col min="6" max="6" width="20.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -1392,22 +1437,61 @@
       <c r="F1" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="G1" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="23">
+        <v>44673</v>
+      </c>
+      <c r="B2" s="0"/>
+      <c r="C2" s="0"/>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="0"/>
+      <c r="G2" s="21">
+        <v>500</v>
+      </c>
+      <c r="H2" s="21">
+        <v>750</v>
+      </c>
+      <c r="I2" s="21">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="24">
+        <v>44673</v>
+      </c>
+      <c r="B3" s="0">
+        <v>350</v>
+      </c>
+      <c r="C3" s="0">
+        <v>350</v>
+      </c>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22">
+        <v>400</v>
+      </c>
+      <c r="I3" s="22">
+        <v>750</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.787402" bottom="0.787402" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
All Transactions Type coded
-get logic for category of expenses and incomes
-define regular transactions
-update liquid and fixed values
-update income sheet
</commit_message>
<xml_diff>
--- a/exe/2022_FinancialRecords.xlsx
+++ b/exe/2022_FinancialRecords.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>Category</t>
   </si>
@@ -126,6 +126,33 @@
   </si>
   <si>
     <t>Allocation</t>
+  </si>
+  <si>
+    <t>Ralekin</t>
+  </si>
+  <si>
+    <t>Liquid</t>
+  </si>
+  <si>
+    <t>Metona</t>
+  </si>
+  <si>
+    <t>Generat</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Meyco</t>
+  </si>
+  <si>
+    <t>Veranda</t>
+  </si>
+  <si>
+    <t>Valkyrie</t>
+  </si>
+  <si>
+    <t>Fixed Asset</t>
   </si>
 </sst>
 </file>
@@ -1038,7 +1065,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
@@ -1103,40 +1130,137 @@
       <c r="K2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
+      <c r="M2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="5">
+        <v>2250</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="A3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1500</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1500</v>
+      </c>
+      <c r="E3" s="5">
+        <f>D3-C3</f>
+      </c>
       <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="5">
+        <v>35.5</v>
+      </c>
+      <c r="I3" s="5">
+        <v>798.75</v>
+      </c>
+      <c r="J3" s="5">
+        <v>798.75</v>
+      </c>
+      <c r="K3" s="5">
+        <f>J3-I3</f>
+      </c>
       <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
+      <c r="M3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" s="5">
+        <v>4500</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="A4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="5">
+        <v>750</v>
+      </c>
+      <c r="D4" s="5">
+        <v>750</v>
+      </c>
+      <c r="E4" s="5">
+        <f>D4-C4</f>
+      </c>
       <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4">
+        <v>22.25</v>
+      </c>
+      <c r="I4">
+        <v>500.625</v>
+      </c>
+      <c r="J4">
+        <v>500.625</v>
+      </c>
+      <c r="K4">
+        <f>J4-I4</f>
+      </c>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5">
+        <v>4500</v>
+      </c>
+      <c r="D5">
+        <v>4500</v>
+      </c>
+      <c r="E5">
+        <f>D5-C5</f>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5">
+        <v>42.25</v>
+      </c>
+      <c r="I5">
+        <v>950.625</v>
+      </c>
+      <c r="J5">
+        <v>950.625</v>
+      </c>
+      <c r="K5">
+        <f>J5-I5</f>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6">
+        <v>100</v>
+      </c>
+      <c r="I6">
+        <v>4500</v>
+      </c>
+      <c r="J6">
+        <v>4500</v>
+      </c>
+      <c r="K6">
+        <f>J6-I6</f>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>